<commit_message>
Fixed room overloading (not sort event)
</commit_message>
<xml_diff>
--- a/DATA/DATA Converter.xlsx
+++ b/DATA/DATA Converter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\SE-Vaerelser\SE-weekend-vaerelser\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{82900707-5AEA-44BD-87E3-60C269B62F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D974A8C4-B96F-43EF-A380-CE6BAC07352F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="1080" windowWidth="21600" windowHeight="12645" activeTab="2" xr2:uid="{924A6A39-D801-4948-B54D-D837DE68D1A9}"/>
+    <workbookView xWindow="1575" yWindow="1230" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{924A6A39-D801-4948-B54D-D837DE68D1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="CALC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -1585,7 +1584,7 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1658,7 @@
         <v>274</v>
       </c>
       <c r="G3" s="1">
-        <v>101012020</v>
+        <v>101012021</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3522,7 +3521,7 @@
         <v>47</v>
       </c>
       <c r="G84" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3545,7 +3544,7 @@
         <v>43</v>
       </c>
       <c r="G85" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3568,7 +3567,7 @@
         <v>39</v>
       </c>
       <c r="G86" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3591,7 +3590,7 @@
         <v>35</v>
       </c>
       <c r="G87" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3614,7 +3613,7 @@
         <v>32</v>
       </c>
       <c r="G88" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3637,7 +3636,7 @@
         <v>28</v>
       </c>
       <c r="G89" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3683,7 +3682,7 @@
         <v>20</v>
       </c>
       <c r="G91" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3706,7 +3705,7 @@
         <v>16</v>
       </c>
       <c r="G92" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4005,7 +4004,7 @@
         <v>184</v>
       </c>
       <c r="G105" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4097,7 +4096,7 @@
         <v>173</v>
       </c>
       <c r="G109" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4143,7 +4142,7 @@
         <v>205</v>
       </c>
       <c r="G111" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4189,7 +4188,7 @@
         <v>161</v>
       </c>
       <c r="G113" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4212,7 +4211,7 @@
         <v>31</v>
       </c>
       <c r="G114" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4396,7 +4395,7 @@
         <v>136</v>
       </c>
       <c r="G122" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -4419,7 +4418,7 @@
         <v>133</v>
       </c>
       <c r="G123" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -4442,7 +4441,7 @@
         <v>130</v>
       </c>
       <c r="G124" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -4465,7 +4464,7 @@
         <v>346</v>
       </c>
       <c r="G125" s="1">
-        <v>101012021</v>
+        <v>101012020</v>
       </c>
     </row>
   </sheetData>
@@ -4480,8 +4479,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1562EB-05F8-4C1F-B172-439FB6B994E1}">
   <dimension ref="A1:M136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4557,7 @@
       </c>
       <c r="F3" t="str">
         <f>IF(ISEVEN(DATA!G3),"f","m")</f>
-        <v>f</v>
+        <v>m</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -6340,7 +6339,7 @@
       </c>
       <c r="F84" t="str">
         <f>IF(ISEVEN(DATA!G84),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -6362,7 +6361,7 @@
       </c>
       <c r="F85" t="str">
         <f>IF(ISEVEN(DATA!G85),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -6384,7 +6383,7 @@
       </c>
       <c r="F86" t="str">
         <f>IF(ISEVEN(DATA!G86),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -6406,7 +6405,7 @@
       </c>
       <c r="F87" t="str">
         <f>IF(ISEVEN(DATA!G87),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -6428,7 +6427,7 @@
       </c>
       <c r="F88" t="str">
         <f>IF(ISEVEN(DATA!G88),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -6450,7 +6449,7 @@
       </c>
       <c r="F89" t="str">
         <f>IF(ISEVEN(DATA!G89),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -6494,7 +6493,7 @@
       </c>
       <c r="F91" t="str">
         <f>IF(ISEVEN(DATA!G91),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -6516,7 +6515,7 @@
       </c>
       <c r="F92" t="str">
         <f>IF(ISEVEN(DATA!G92),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -6802,7 +6801,7 @@
       </c>
       <c r="F105" t="str">
         <f>IF(ISEVEN(DATA!G105),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -6890,7 +6889,7 @@
       </c>
       <c r="F109" t="str">
         <f>IF(ISEVEN(DATA!G109),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -6934,7 +6933,7 @@
       </c>
       <c r="F111" t="str">
         <f>IF(ISEVEN(DATA!G111),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -6978,7 +6977,7 @@
       </c>
       <c r="F113" t="str">
         <f>IF(ISEVEN(DATA!G113),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -7000,7 +6999,7 @@
       </c>
       <c r="F114" t="str">
         <f>IF(ISEVEN(DATA!G114),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -7176,7 +7175,7 @@
       </c>
       <c r="F122" t="str">
         <f>IF(ISEVEN(DATA!G122),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -7198,7 +7197,7 @@
       </c>
       <c r="F123" t="str">
         <f>IF(ISEVEN(DATA!G123),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -7220,7 +7219,7 @@
       </c>
       <c r="F124" t="str">
         <f>IF(ISEVEN(DATA!G124),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -7242,7 +7241,7 @@
       </c>
       <c r="F125" t="str">
         <f>IF(ISEVEN(DATA!G125),"f","m")</f>
-        <v>m</v>
+        <v>f</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -7496,7 +7495,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6FC552-D7C7-4211-9C63-BA1F0E8C637B}">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -9250,6 +9249,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="97135ab5-73c1-4618-8fe0-3cb2e310caa6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010028590748EF5E6542A97F9AB6CFBBF597" ma:contentTypeVersion="8" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="ffe9c388d0e6edf31ef03a66fa7c6455">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="97135ab5-73c1-4618-8fe0-3cb2e310caa6" xmlns:ns4="e22c8b26-ef4b-4e69-b083-d3df374cb404" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b0097434470845424b25098c4c0cd69" ns3:_="" ns4:_="">
     <xsd:import namespace="97135ab5-73c1-4618-8fe0-3cb2e310caa6"/>
@@ -9438,24 +9454,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="97135ab5-73c1-4618-8fe0-3cb2e310caa6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{9D34E11B-46CD-4182-823F-0B565DAD76D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{54784413-D600-4BA5-845F-24FCF019E15B}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{E6386EF1-0CCD-4C0B-BC43-41690C0A6C5C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9472,18 +9485,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{54784413-D600-4BA5-845F-24FCF019E15B}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{9D34E11B-46CD-4182-823F-0B565DAD76D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>